<commit_message>
feat: add thermal printer support and update product IDs
- Added `node-thermal-printer` dependency for printing receipts.
- Implemented `PrinterHandler` to manage printing receipts with MPR-200.
- Updated `server.js` to handle printing requests during sales.
- Modified `script.js` to synchronize product lists and handle local product loading.
- Migrated product IDs in `productos_inventario.json` to UUID format.
- Created scripts for listing products and migrating IDs from Excel to JSON.
- Updated `productos_inventario.json` with new UUIDs for all products.
- Enhanced error handling and logging for printing and migration processes.
</commit_message>
<xml_diff>
--- a/data/cafe_data.xlsx
+++ b/data/cafe_data.xlsx
@@ -400,9 +400,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -428,18 +428,1581 @@
         <v>minStock</v>
       </c>
       <c r="H1" t="str">
-        <v>image</v>
+        <v>createdAt</v>
       </c>
       <c r="I1" t="str">
-        <v>createdAt</v>
-      </c>
-      <c r="J1" t="str">
         <v>updatedAt</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Café Helado</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Café Helado</v>
+      </c>
+      <c r="D2" t="str">
+        <v>bebidas</v>
+      </c>
+      <c r="E2">
+        <v>6000</v>
+      </c>
+      <c r="F2">
+        <v>197</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2025-09-04T01:31:55.815Z</v>
+      </c>
+      <c r="I2" t="str">
+        <v>2025-09-04T03:27:07.595Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>ff9086e4-ebac-4ff0-b970-8979605da5b0</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Maracuyazo</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Maracuya con helado</v>
+      </c>
+      <c r="D3" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E3">
+        <v>10000</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3" t="str">
+        <v>2025-09-04T01:33:11.725Z</v>
+      </c>
+      <c r="I3" t="str">
+        <v>2025-09-04T02:51:46.475Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>6c71bdee-433a-435c-85ba-8e346ab1ac15</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Capuccino</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Capuccino</v>
+      </c>
+      <c r="D4" t="str">
+        <v>bebidas</v>
+      </c>
+      <c r="E4">
+        <v>8000</v>
+      </c>
+      <c r="F4">
+        <v>200</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4" t="str">
+        <v>2025-09-04T02:37:49.920Z</v>
+      </c>
+      <c r="I4" t="str">
+        <v>2025-09-04T02:37:49.920Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>6d7cd20c-f927-4f4f-95e8-44a7b5f73e56</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Mocacino</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Mocacino</v>
+      </c>
+      <c r="D5" t="str">
+        <v>bebidas</v>
+      </c>
+      <c r="E5">
+        <v>6000</v>
+      </c>
+      <c r="F5">
+        <v>200</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5" t="str">
+        <v>2025-09-04T02:37:49.929Z</v>
+      </c>
+      <c r="I5" t="str">
+        <v>2025-09-04T02:38:07.394Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>915bb3d8-08d2-4fe5-87d6-09b38b2fa4cd</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Café Latte</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Café Latte</v>
+      </c>
+      <c r="D6" t="str">
+        <v>bebidas</v>
+      </c>
+      <c r="E6">
+        <v>8000</v>
+      </c>
+      <c r="F6">
+        <v>199</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6" t="str">
+        <v>2025-09-04T02:37:49.938Z</v>
+      </c>
+      <c r="I6" t="str">
+        <v>2025-09-04T02:56:08.469Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>8f13be85-8476-4e66-a65a-a34cf2299370</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Americano</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Americano</v>
+      </c>
+      <c r="D7" t="str">
+        <v>bebidas</v>
+      </c>
+      <c r="E7">
+        <v>8000</v>
+      </c>
+      <c r="F7">
+        <v>200</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7" t="str">
+        <v>2025-09-04T02:37:49.947Z</v>
+      </c>
+      <c r="I7" t="str">
+        <v>2025-09-04T02:37:49.947Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>cb79e58b-5fc9-4887-8fae-53c3070ed207</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Expresso</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Expresso</v>
+      </c>
+      <c r="D8" t="str">
+        <v>bebidas</v>
+      </c>
+      <c r="E8">
+        <v>8000</v>
+      </c>
+      <c r="F8">
+        <v>200</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8" t="str">
+        <v>2025-09-04T02:37:49.954Z</v>
+      </c>
+      <c r="I8" t="str">
+        <v>2025-09-04T02:37:49.954Z</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>3615f380-3601-4397-a723-637c5496f99e</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Aromática Frutos</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Aromática Frutos</v>
+      </c>
+      <c r="D9" t="str">
+        <v>bebidas</v>
+      </c>
+      <c r="E9">
+        <v>8000</v>
+      </c>
+      <c r="F9">
+        <v>200</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9" t="str">
+        <v>2025-09-04T02:37:49.962Z</v>
+      </c>
+      <c r="I9" t="str">
+        <v>2025-09-04T02:37:49.962Z</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>11bb2e58-53c5-428f-9e53-0d8db165f136</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Chocolate</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Chocolate</v>
+      </c>
+      <c r="D10" t="str">
+        <v>bebidas</v>
+      </c>
+      <c r="E10">
+        <v>8000</v>
+      </c>
+      <c r="F10">
+        <v>200</v>
+      </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10" t="str">
+        <v>2025-09-04T02:37:49.970Z</v>
+      </c>
+      <c r="I10" t="str">
+        <v>2025-09-04T02:37:49.970Z</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>3b9f84fe-174e-47bc-a951-11eb71b0a556</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Jugo Natural</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Jugo Natural</v>
+      </c>
+      <c r="D11" t="str">
+        <v>bebidas</v>
+      </c>
+      <c r="E11">
+        <v>8000</v>
+      </c>
+      <c r="F11">
+        <v>200</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11" t="str">
+        <v>2025-09-04T02:37:49.979Z</v>
+      </c>
+      <c r="I11" t="str">
+        <v>2025-09-04T02:37:49.979Z</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>29abc6c8-a28b-4859-906e-121bf7a8f657</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Cerveza Budweiser</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Cerveza Budweiser</v>
+      </c>
+      <c r="D12" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E12">
+        <v>8000</v>
+      </c>
+      <c r="F12">
+        <v>30</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12" t="str">
+        <v>2025-09-04T02:37:49.987Z</v>
+      </c>
+      <c r="I12" t="str">
+        <v>2025-09-04T02:37:49.987Z</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>bb1eb308-876d-4d78-b1c0-6473704c3cc0</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Cerveza Pilsen Latón</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Cerveza Pilsen Latón</v>
+      </c>
+      <c r="D13" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E13">
+        <v>6000</v>
+      </c>
+      <c r="F13">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" t="str">
+        <v>2025-09-04T02:37:49.995Z</v>
+      </c>
+      <c r="I13" t="str">
+        <v>2025-09-04T02:37:49.995Z</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>5d4c78f0-98ed-4619-8bab-f926ebf0b8f3</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Cerveza Bitburger</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Cerveza Bitburger</v>
+      </c>
+      <c r="D14" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E14">
+        <v>6000</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14" t="str">
+        <v>2025-09-04T02:37:50.003Z</v>
+      </c>
+      <c r="I14" t="str">
+        <v>2025-09-04T02:37:50.003Z</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>a833bd69-0b44-4491-92d1-1a02b164441c</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Cerveza BBC Rose</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Cerveza BBC Rose</v>
+      </c>
+      <c r="D15" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E15">
+        <v>3500</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15" t="str">
+        <v>2025-09-04T02:37:50.010Z</v>
+      </c>
+      <c r="I15" t="str">
+        <v>2025-09-04T02:37:50.010Z</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>60ca7511-1787-4f23-bb4f-bb645e745d63</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Cerveza BCC Miel</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Cerveza BCC Miel</v>
+      </c>
+      <c r="D16" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E16">
+        <v>2500</v>
+      </c>
+      <c r="F16">
+        <v>30</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16" t="str">
+        <v>2025-09-04T02:37:50.019Z</v>
+      </c>
+      <c r="I16" t="str">
+        <v>2025-09-04T02:37:50.019Z</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>7a9a2a17-b550-4611-b032-438fe36ad898</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Club Colombia Dorada</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Club Colombia Dorada</v>
+      </c>
+      <c r="D17" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E17">
+        <v>2500</v>
+      </c>
+      <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17" t="str">
+        <v>2025-09-04T02:37:50.027Z</v>
+      </c>
+      <c r="I17" t="str">
+        <v>2025-09-04T02:37:50.027Z</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>52b56fd6-1496-4370-8a11-e524aada7f7a</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Cerveza Aguila Original</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Cerveza Aguila Original</v>
+      </c>
+      <c r="D18" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E18">
+        <v>3500</v>
+      </c>
+      <c r="F18">
+        <v>30</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18" t="str">
+        <v>2025-09-04T02:37:50.037Z</v>
+      </c>
+      <c r="I18" t="str">
+        <v>2025-09-04T02:37:50.037Z</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>21400f6a-8760-49ba-9514-5cea4c8abfcb</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Cerveza Corona Extra</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Cerveza Corona Extra</v>
+      </c>
+      <c r="D19" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E19">
+        <v>4000</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19" t="str">
+        <v>2025-09-04T02:37:50.045Z</v>
+      </c>
+      <c r="I19" t="str">
+        <v>2025-09-04T02:37:50.045Z</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>490c05bf-ff93-4674-8031-32eaeb05342f</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Cerveza Stella</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Cerveza Stella</v>
+      </c>
+      <c r="D20" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E20">
+        <v>5000</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20" t="str">
+        <v>2025-09-04T02:37:50.052Z</v>
+      </c>
+      <c r="I20" t="str">
+        <v>2025-09-04T02:37:50.052Z</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>53a19032-962f-4fa1-bb4c-9ab69a496262</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Cerveza Heineken</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Cerveza Heineken</v>
+      </c>
+      <c r="D21" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E21">
+        <v>6000</v>
+      </c>
+      <c r="F21">
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21" t="str">
+        <v>2025-09-04T02:37:50.060Z</v>
+      </c>
+      <c r="I21" t="str">
+        <v>2025-09-04T02:37:50.060Z</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>a5081127-bfff-4142-a625-6831690ebde6</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Cerveza Redds</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Cerveza Redds</v>
+      </c>
+      <c r="D22" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E22">
+        <v>6000</v>
+      </c>
+      <c r="F22">
+        <v>30</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22" t="str">
+        <v>2025-09-04T02:37:50.068Z</v>
+      </c>
+      <c r="I22" t="str">
+        <v>2025-09-04T02:37:50.068Z</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>d83aa662-74c0-41fd-a4f2-9fb7577d7b2d</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Cerveza Peroni</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Cerveza Peroni</v>
+      </c>
+      <c r="D23" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E23">
+        <v>6000</v>
+      </c>
+      <c r="F23">
+        <v>30</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23" t="str">
+        <v>2025-09-04T02:37:50.076Z</v>
+      </c>
+      <c r="I23" t="str">
+        <v>2025-09-04T02:37:50.076Z</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>6b1f9691-fffd-4ce3-9a43-4c51d4cb4084</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Cerveza Andina</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Cerveza Andina</v>
+      </c>
+      <c r="D24" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E24">
+        <v>5000</v>
+      </c>
+      <c r="F24">
+        <v>30</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24" t="str">
+        <v>2025-09-04T02:37:50.085Z</v>
+      </c>
+      <c r="I24" t="str">
+        <v>2025-09-04T02:37:50.085Z</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>1432667b-8f08-41a5-92b0-d52cba2e109e</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Cerveza Andina Light</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Cerveza Andina Light</v>
+      </c>
+      <c r="D25" t="str">
+        <v>cervezas</v>
+      </c>
+      <c r="E25">
+        <v>5000</v>
+      </c>
+      <c r="F25">
+        <v>30</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25" t="str">
+        <v>2025-09-04T02:37:50.094Z</v>
+      </c>
+      <c r="I25" t="str">
+        <v>2025-09-04T02:37:50.094Z</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>2ca50846-3c11-4a43-92a2-0cf175480254</v>
+      </c>
+      <c r="B26" t="str">
+        <v>HIDRA TAO</v>
+      </c>
+      <c r="C26" t="str">
+        <v>HIDRA TAO</v>
+      </c>
+      <c r="D26" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E26">
+        <v>7000</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" t="str">
+        <v>2025-09-04T02:37:50.102Z</v>
+      </c>
+      <c r="I26" t="str">
+        <v>2025-09-04T02:37:50.102Z</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>8bd328a8-e5bd-4eb3-9d80-0476acee1b48</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Gatorade</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Gatorade</v>
+      </c>
+      <c r="D27" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E27">
+        <v>7000</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27" t="str">
+        <v>2025-09-04T02:37:50.110Z</v>
+      </c>
+      <c r="I27" t="str">
+        <v>2025-09-04T02:37:50.110Z</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>0f60b7c8-6b34-4588-b3a8-f2aadb4ddb42</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Electrolit</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Electrolit</v>
+      </c>
+      <c r="D28" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E28">
+        <v>15000</v>
+      </c>
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28" t="str">
+        <v>2025-09-04T02:37:50.117Z</v>
+      </c>
+      <c r="I28" t="str">
+        <v>2025-09-04T02:37:50.117Z</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>c772260d-e3f7-4601-b8c1-a1e11e29e8a3</v>
+      </c>
+      <c r="B29" t="str">
+        <v>FOUR LOKO</v>
+      </c>
+      <c r="C29" t="str">
+        <v>FOUR LOKO</v>
+      </c>
+      <c r="D29" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E29">
+        <v>8000</v>
+      </c>
+      <c r="F29">
+        <v>30</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29" t="str">
+        <v>2025-09-04T02:37:50.125Z</v>
+      </c>
+      <c r="I29" t="str">
+        <v>2025-09-04T02:37:50.125Z</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>e3f4854f-2591-4ec1-8137-384098e55ac2</v>
+      </c>
+      <c r="B30" t="str">
+        <v>JP</v>
+      </c>
+      <c r="C30" t="str">
+        <v>JP</v>
+      </c>
+      <c r="D30" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E30">
+        <v>8000</v>
+      </c>
+      <c r="F30">
+        <v>30</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30" t="str">
+        <v>2025-09-04T02:37:50.132Z</v>
+      </c>
+      <c r="I30" t="str">
+        <v>2025-09-04T02:37:50.132Z</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>ba97a098-7926-4bef-895a-9f9b012b1063</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Cuba Libre Ron y Coca Cola</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Cuba Libre Ron y Coca Cola</v>
+      </c>
+      <c r="D31" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E31">
+        <v>6000</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31" t="str">
+        <v>2025-09-04T02:37:50.139Z</v>
+      </c>
+      <c r="I31" t="str">
+        <v>2025-09-04T02:37:50.139Z</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>d1b02028-cbe1-43b1-b587-30ac5b80d634</v>
+      </c>
+      <c r="B32" t="str">
+        <v>CUBA LIBRE MOJITO de ron viejo de caldas</v>
+      </c>
+      <c r="C32" t="str">
+        <v>CUBA LIBRE MOJITO de ron viejo de caldas</v>
+      </c>
+      <c r="D32" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E32">
+        <v>6000</v>
+      </c>
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="H32" t="str">
+        <v>2025-09-04T02:37:50.147Z</v>
+      </c>
+      <c r="I32" t="str">
+        <v>2025-09-04T02:37:50.147Z</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>4bc5e62f-204a-414e-a78a-9dcd96e123a9</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Smirnoff</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Smirnoff</v>
+      </c>
+      <c r="D33" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E33">
+        <v>6500</v>
+      </c>
+      <c r="F33">
+        <v>30</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33" t="str">
+        <v>2025-09-04T02:37:50.155Z</v>
+      </c>
+      <c r="I33" t="str">
+        <v>2025-09-04T02:37:50.155Z</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>93808860-76b0-455c-be8b-974b2ad82dd8</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Redubull</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Redubull</v>
+      </c>
+      <c r="D34" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E34">
+        <v>7000</v>
+      </c>
+      <c r="F34">
+        <v>30</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34" t="str">
+        <v>2025-09-04T02:37:50.162Z</v>
+      </c>
+      <c r="I34" t="str">
+        <v>2025-09-04T02:37:50.162Z</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>586d913e-286a-444d-aa9e-a5189272d913</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Agua Brisa Saborizada</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Agua Brisa Saborizada</v>
+      </c>
+      <c r="D35" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E35">
+        <v>6500</v>
+      </c>
+      <c r="F35">
+        <v>30</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35" t="str">
+        <v>2025-09-04T02:37:50.170Z</v>
+      </c>
+      <c r="I35" t="str">
+        <v>2025-09-04T02:37:50.170Z</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>3153a658-8332-45e8-8d4d-463bb5d3aaff</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Agua sin Gas Manantial</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Agua sin Gas Manantial</v>
+      </c>
+      <c r="D36" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E36">
+        <v>6000</v>
+      </c>
+      <c r="F36">
+        <v>30</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36" t="str">
+        <v>2025-09-04T02:37:50.177Z</v>
+      </c>
+      <c r="I36" t="str">
+        <v>2025-09-04T02:37:50.177Z</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>41078390-38e8-4f47-8e06-a2e85de4e90b</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Hatsu Té</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Hatsu Té</v>
+      </c>
+      <c r="D37" t="str">
+        <v>liquidos</v>
+      </c>
+      <c r="E37">
+        <v>8000</v>
+      </c>
+      <c r="F37">
+        <v>30</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37" t="str">
+        <v>2025-09-04T02:37:50.186Z</v>
+      </c>
+      <c r="I37" t="str">
+        <v>2025-09-04T02:37:50.186Z</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>850c1eaa-ec98-4238-82c0-d2ee4e249121</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Paquete Papas</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Paquete Papas</v>
+      </c>
+      <c r="D38" t="str">
+        <v>snacks</v>
+      </c>
+      <c r="E38">
+        <v>8000</v>
+      </c>
+      <c r="F38">
+        <v>30</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38" t="str">
+        <v>2025-09-04T02:37:50.195Z</v>
+      </c>
+      <c r="I38" t="str">
+        <v>2025-09-04T02:37:50.195Z</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>7e8be0bd-663d-4755-ad65-cdb9bce26c6f</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Producto 6000</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Producto 6000</v>
+      </c>
+      <c r="D39" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E39">
+        <v>6000</v>
+      </c>
+      <c r="F39">
+        <v>30</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+      <c r="H39" t="str">
+        <v>2025-09-04T02:37:50.203Z</v>
+      </c>
+      <c r="I39" t="str">
+        <v>2025-09-04T02:37:50.203Z</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>1624e55b-cb11-4c1d-b678-955589c1d300</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Producto 12000</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Producto 12000</v>
+      </c>
+      <c r="D40" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E40">
+        <v>12000</v>
+      </c>
+      <c r="F40">
+        <v>30</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="H40" t="str">
+        <v>2025-09-04T02:37:50.211Z</v>
+      </c>
+      <c r="I40" t="str">
+        <v>2025-09-04T02:37:50.211Z</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>ccbda64f-503e-41fe-8558-b42fb041626e</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Producto 20000</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Producto 20000</v>
+      </c>
+      <c r="D41" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E41">
+        <v>20000</v>
+      </c>
+      <c r="F41">
+        <v>30</v>
+      </c>
+      <c r="G41">
+        <v>5</v>
+      </c>
+      <c r="H41" t="str">
+        <v>2025-09-04T02:37:50.219Z</v>
+      </c>
+      <c r="I41" t="str">
+        <v>2025-09-04T02:37:50.220Z</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>b313fc3e-7f05-4adb-942b-0a82117906b7</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Producto 15000</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Producto 15000</v>
+      </c>
+      <c r="D42" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E42">
+        <v>15000</v>
+      </c>
+      <c r="F42">
+        <v>30</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="H42" t="str">
+        <v>2025-09-04T02:37:50.229Z</v>
+      </c>
+      <c r="I42" t="str">
+        <v>2025-09-04T02:37:50.229Z</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>0059b86f-f5e5-45d5-8a07-193237a2a702</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Producto 15000</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Producto 15000</v>
+      </c>
+      <c r="D43" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E43">
+        <v>15000</v>
+      </c>
+      <c r="F43">
+        <v>30</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+      <c r="H43" t="str">
+        <v>2025-09-04T02:37:50.237Z</v>
+      </c>
+      <c r="I43" t="str">
+        <v>2025-09-04T02:37:50.237Z</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>b2a5704c-ac36-408d-87ae-ba04363db0dc</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Producto 15000</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Producto 15000</v>
+      </c>
+      <c r="D44" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E44">
+        <v>15000</v>
+      </c>
+      <c r="F44">
+        <v>30</v>
+      </c>
+      <c r="G44">
+        <v>5</v>
+      </c>
+      <c r="H44" t="str">
+        <v>2025-09-04T02:37:50.244Z</v>
+      </c>
+      <c r="I44" t="str">
+        <v>2025-09-04T02:37:50.244Z</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>a6e62d4f-2e39-4140-ab96-dc16889d0590</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Producto 11000</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Producto 11000</v>
+      </c>
+      <c r="D45" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E45">
+        <v>11000</v>
+      </c>
+      <c r="F45">
+        <v>30</v>
+      </c>
+      <c r="G45">
+        <v>5</v>
+      </c>
+      <c r="H45" t="str">
+        <v>2025-09-04T02:37:50.253Z</v>
+      </c>
+      <c r="I45" t="str">
+        <v>2025-09-04T02:37:50.253Z</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>5fcab383-6ba4-4610-82b9-d99bf6d055b2</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Producto 2500</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Producto 2500</v>
+      </c>
+      <c r="D46" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E46">
+        <v>2500</v>
+      </c>
+      <c r="F46">
+        <v>30</v>
+      </c>
+      <c r="G46">
+        <v>5</v>
+      </c>
+      <c r="H46" t="str">
+        <v>2025-09-04T02:37:50.260Z</v>
+      </c>
+      <c r="I46" t="str">
+        <v>2025-09-04T02:37:50.260Z</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>27318288-7346-4d3b-9ddd-aa90106d9a14</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Producto 7000</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Producto 7000</v>
+      </c>
+      <c r="D47" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E47">
+        <v>7000</v>
+      </c>
+      <c r="F47">
+        <v>30</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+      <c r="H47" t="str">
+        <v>2025-09-04T02:37:50.268Z</v>
+      </c>
+      <c r="I47" t="str">
+        <v>2025-09-04T02:37:50.268Z</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>3ef67109-1e6a-4065-a80e-2ada028282ea</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Producto 4000</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Producto 4000</v>
+      </c>
+      <c r="D48" t="str">
+        <v>otros</v>
+      </c>
+      <c r="E48">
+        <v>4000</v>
+      </c>
+      <c r="F48">
+        <v>30</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48" t="str">
+        <v>2025-09-04T02:37:50.276Z</v>
+      </c>
+      <c r="I48" t="str">
+        <v>2025-09-04T02:37:50.276Z</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>bf00d70d-5b63-4cc8-8014-8d4df62d3efa</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Paquete x12</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Paquete x12</v>
+      </c>
+      <c r="D49" t="str">
+        <v>chocolates_cafe</v>
+      </c>
+      <c r="E49">
+        <v>28000</v>
+      </c>
+      <c r="F49">
+        <v>40</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49" t="str">
+        <v>2025-09-04T02:37:50.283Z</v>
+      </c>
+      <c r="I49" t="str">
+        <v>2025-09-04T02:37:50.283Z</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>4b7d81e8-3e81-436a-8e23-f72ec5d95603</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Unidad x4 Chocolates</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Unidad x4 Chocolates</v>
+      </c>
+      <c r="D50" t="str">
+        <v>chocolates_cafe</v>
+      </c>
+      <c r="E50">
+        <v>3000</v>
+      </c>
+      <c r="F50">
+        <v>40</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50" t="str">
+        <v>2025-09-04T02:37:50.293Z</v>
+      </c>
+      <c r="I50" t="str">
+        <v>2025-09-04T02:37:50.293Z</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>da35c3dc-0067-43e1-bdba-997d1413b49c</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Unidad x10 Chocolates</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Unidad x10 Chocolates</v>
+      </c>
+      <c r="D51" t="str">
+        <v>chocolates_cafe</v>
+      </c>
+      <c r="E51">
+        <v>7000</v>
+      </c>
+      <c r="F51">
+        <v>40</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51" t="str">
+        <v>2025-09-04T02:37:50.301Z</v>
+      </c>
+      <c r="I51" t="str">
+        <v>2025-09-04T02:37:50.301Z</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>fec660e6-4f94-464e-8317-33703b793bee</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Chocolatina</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Chocolatina</v>
+      </c>
+      <c r="D52" t="str">
+        <v>chocolates_cafe</v>
+      </c>
+      <c r="E52">
+        <v>7000</v>
+      </c>
+      <c r="F52">
+        <v>40</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52" t="str">
+        <v>2025-09-04T02:37:50.309Z</v>
+      </c>
+      <c r="I52" t="str">
+        <v>2025-09-04T02:37:50.309Z</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>324f9fd6-5a5c-4ec2-b8ec-4b572bd46951</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Café 125g</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Café 125g</v>
+      </c>
+      <c r="D53" t="str">
+        <v>chocolates_cafe</v>
+      </c>
+      <c r="E53">
+        <v>15000</v>
+      </c>
+      <c r="F53">
+        <v>50</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53" t="str">
+        <v>2025-09-04T02:37:50.317Z</v>
+      </c>
+      <c r="I53" t="str">
+        <v>2025-09-04T02:37:50.317Z</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>c1725de0-db41-42f7-bb0d-e7af725c541a</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Café 250g</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Café 250g</v>
+      </c>
+      <c r="D54" t="str">
+        <v>chocolates_cafe</v>
+      </c>
+      <c r="E54">
+        <v>24000</v>
+      </c>
+      <c r="F54">
+        <v>50</v>
+      </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
+      <c r="H54" t="str">
+        <v>2025-09-04T02:37:50.325Z</v>
+      </c>
+      <c r="I54" t="str">
+        <v>2025-09-04T02:37:50.325Z</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>b4f544af-8b69-4ab3-a070-f038de225e0a</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Café 500g</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Café 500g</v>
+      </c>
+      <c r="D55" t="str">
+        <v>chocolates_cafe</v>
+      </c>
+      <c r="E55">
+        <v>42000</v>
+      </c>
+      <c r="F55">
+        <v>50</v>
+      </c>
+      <c r="G55">
+        <v>5</v>
+      </c>
+      <c r="H55" t="str">
+        <v>2025-09-04T02:37:50.333Z</v>
+      </c>
+      <c r="I55" t="str">
+        <v>2025-09-04T02:37:50.333Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I55"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -448,7 +2011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -489,9 +2052,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -514,18 +2077,86 @@
         <v>createdAt</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>94edc518-f3e0-4000-9c1a-6395c71e28ad</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Cliente General</v>
+      </c>
+      <c r="D2">
+        <v>6000</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2025-09-04T02:40:25.668Z</v>
+      </c>
+      <c r="F2" t="str">
+        <v>2025-09-04T02:40:25.668Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>5691be93-db36-47f8-9708-21470050bd84</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Cliente General</v>
+      </c>
+      <c r="D3">
+        <v>8000</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2025-09-04T02:56:08.452Z</v>
+      </c>
+      <c r="F3" t="str">
+        <v>2025-09-04T02:56:08.452Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>4e7d358b-4278-48ff-b74d-77a6c5fe2c36</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Cliente General</v>
+      </c>
+      <c r="D4">
+        <v>6000</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2025-09-04T03:08:42.564Z</v>
+      </c>
+      <c r="F4" t="str">
+        <v>2025-09-04T03:08:42.564Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2cea67ab-bca9-4a36-bc74-b40d50d02de3</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Cliente General</v>
+      </c>
+      <c r="D5">
+        <v>6000</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2025-09-04T03:27:07.571Z</v>
+      </c>
+      <c r="F5" t="str">
+        <v>2025-09-04T03:27:07.571Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -551,9 +2182,101 @@
         <v>subtotal</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>94edc518-f3e0-4000-9c1a-6395c71e28ad_2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="B2" t="str">
+        <v>94edc518-f3e0-4000-9c1a-6395c71e28ad</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Café Helado</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>6000</v>
+      </c>
+      <c r="G2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>5691be93-db36-47f8-9708-21470050bd84_915bb3d8-08d2-4fe5-87d6-09b38b2fa4cd</v>
+      </c>
+      <c r="B3" t="str">
+        <v>5691be93-db36-47f8-9708-21470050bd84</v>
+      </c>
+      <c r="C3" t="str">
+        <v>915bb3d8-08d2-4fe5-87d6-09b38b2fa4cd</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Café Latte</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>8000</v>
+      </c>
+      <c r="G3">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>4e7d358b-4278-48ff-b74d-77a6c5fe2c36_2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="B4" t="str">
+        <v>4e7d358b-4278-48ff-b74d-77a6c5fe2c36</v>
+      </c>
+      <c r="C4" t="str">
+        <v>2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Café Helado</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>6000</v>
+      </c>
+      <c r="G4">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2cea67ab-bca9-4a36-bc74-b40d50d02de3_2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2cea67ab-bca9-4a36-bc74-b40d50d02de3</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Café Helado</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>6000</v>
+      </c>
+      <c r="G5">
+        <v>6000</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: update printer handler import and modify button styles in index.html
</commit_message>
<xml_diff>
--- a/data/cafe_data.xlsx
+++ b/data/cafe_data.xlsx
@@ -448,10 +448,10 @@
         <v>bebidas</v>
       </c>
       <c r="E2">
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="F2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G2">
         <v>20</v>
@@ -460,7 +460,7 @@
         <v>2025-09-04T01:31:55.815Z</v>
       </c>
       <c r="I2" t="str">
-        <v>2025-09-04T03:27:07.595Z</v>
+        <v>2025-09-04T21:18:57.812Z</v>
       </c>
     </row>
     <row r="3">
@@ -2052,7 +2052,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2145,16 +2145,33 @@
         <v>2025-09-04T03:27:07.571Z</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>c82d54ad-d298-4186-b1ab-20aa106d1339</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Cliente General</v>
+      </c>
+      <c r="D6">
+        <v>8000</v>
+      </c>
+      <c r="E6" t="str">
+        <v>2025-09-04T21:18:57.790Z</v>
+      </c>
+      <c r="F6" t="str">
+        <v>2025-09-04T21:18:57.790Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2274,9 +2291,32 @@
         <v>6000</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>c82d54ad-d298-4186-b1ab-20aa106d1339_2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="B6" t="str">
+        <v>c82d54ad-d298-4186-b1ab-20aa106d1339</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Café Helado</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>8000</v>
+      </c>
+      <c r="G6">
+        <v>8000</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: implement receipt printing functionality and enhance sale data structure
</commit_message>
<xml_diff>
--- a/data/cafe_data.xlsx
+++ b/data/cafe_data.xlsx
@@ -451,7 +451,7 @@
         <v>8000</v>
       </c>
       <c r="F2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G2">
         <v>20</v>
@@ -460,7 +460,7 @@
         <v>2025-09-04T01:31:55.815Z</v>
       </c>
       <c r="I2" t="str">
-        <v>2025-09-04T21:18:57.812Z</v>
+        <v>2025-09-06T04:36:07.765Z</v>
       </c>
     </row>
     <row r="3">
@@ -509,7 +509,7 @@
         <v>8000</v>
       </c>
       <c r="F4">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G4">
         <v>20</v>
@@ -518,7 +518,7 @@
         <v>2025-09-04T02:37:49.920Z</v>
       </c>
       <c r="I4" t="str">
-        <v>2025-09-04T02:37:49.920Z</v>
+        <v>2025-09-06T04:26:28.685Z</v>
       </c>
     </row>
     <row r="5">
@@ -2052,7 +2052,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2162,16 +2162,50 @@
         <v>2025-09-04T21:18:57.790Z</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>b5074ae7-6fca-4eb3-8357-cb2d74361718</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Cliente General</v>
+      </c>
+      <c r="D7">
+        <v>8000</v>
+      </c>
+      <c r="E7" t="str">
+        <v>2025-09-06T04:26:28.590Z</v>
+      </c>
+      <c r="F7" t="str">
+        <v>2025-09-06T04:26:28.590Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>09869ab4-f5f0-4f2d-8f99-c81174943ec0</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Cliente General</v>
+      </c>
+      <c r="D8">
+        <v>8000</v>
+      </c>
+      <c r="E8" t="str">
+        <v>2025-09-06T04:36:07.667Z</v>
+      </c>
+      <c r="F8" t="str">
+        <v>2025-09-06T04:36:07.667Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2314,9 +2348,49 @@
         <v>8000</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>b5074ae7-6fca-4eb3-8357-cb2d74361718_6c71bdee-433a-435c-85ba-8e346ab1ac15</v>
+      </c>
+      <c r="B7" t="str">
+        <v>b5074ae7-6fca-4eb3-8357-cb2d74361718</v>
+      </c>
+      <c r="C7" t="str">
+        <v>6c71bdee-433a-435c-85ba-8e346ab1ac15</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>8000</v>
+      </c>
+      <c r="G7">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>09869ab4-f5f0-4f2d-8f99-c81174943ec0_2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="B8" t="str">
+        <v>09869ab4-f5f0-4f2d-8f99-c81174943ec0</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2e23a440-e5e1-4ce2-a407-c15bad1fd402</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>8000</v>
+      </c>
+      <c r="G8">
+        <v>8000</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>